<commit_message>
fix: pertanyaan dan jawaban quiz dengan gambar
</commit_message>
<xml_diff>
--- a/public/FormatImportPertanyaanModul.xlsx
+++ b/public/FormatImportPertanyaanModul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data C\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\e-learning\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF9CC60-E8FB-4453-A344-369AFC8A29D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB9D69-2457-4D17-9F1F-D3EAD962C8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68C48174-30B5-4660-9F37-15C3FC04DB4F}"/>
+    <workbookView xWindow="5250" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{68C48174-30B5-4660-9F37-15C3FC04DB4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -68,18 +68,12 @@
     <t>D</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Kunci Jawaban</t>
   </si>
   <si>
     <t>Jawaban Pilihan ganda</t>
   </si>
   <si>
-    <t>*masukan sesuai format : A = 1, B = 2, C = 3, D = 4, E = 5</t>
-  </si>
-  <si>
     <t>ini jawaban A</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>ini jawaban D</t>
   </si>
   <si>
-    <t>ini jawaban E</t>
-  </si>
-  <si>
     <t>Pilihan Ganda</t>
   </si>
   <si>
@@ -105,6 +96,12 @@
   </si>
   <si>
     <t>FORMAT IMPORT PERTANYAAN MILENIA LEARNING CENTER</t>
+  </si>
+  <si>
+    <t>*masukan sesuai format : A = 1, B = 2, C = 3, D = 4</t>
+  </si>
+  <si>
+    <t>Gambar</t>
   </si>
 </sst>
 </file>
@@ -180,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -302,73 +299,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,6 +433,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E73C410-1835-3A7E-FC4B-780B5DBB9BC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304799" y="1104900"/>
+          <a:ext cx="409575" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -707,271 +804,275 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="3" t="s">
+      <c r="D16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="H16:H17"/>
+  <mergeCells count="19">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="A14:H15"/>
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D9:G11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C9:G11"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A8:H8"/>
     <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: image tidak turun resolusi di excel
</commit_message>
<xml_diff>
--- a/public/FormatImportPertanyaanModul.xlsx
+++ b/public/FormatImportPertanyaanModul.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\e-learning\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB9D69-2457-4D17-9F1F-D3EAD962C8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF95D5B-F48C-483B-B360-7D76BFEBD8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{68C48174-30B5-4660-9F37-15C3FC04DB4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68C48174-30B5-4660-9F37-15C3FC04DB4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -349,6 +349,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -365,57 +416,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,28 +819,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -853,29 +853,29 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
@@ -888,7 +888,7 @@
       <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -939,103 +939,103 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="22" t="s">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="23"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="23"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1048,10 +1048,15 @@
       <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="H17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="D4:G4"/>
@@ -1066,11 +1071,6 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>